<commit_message>
questoes resolvidas e setTopicos
</commit_message>
<xml_diff>
--- a/Provas antigas/PlaniliaQuestoes.xlsx
+++ b/Provas antigas/PlaniliaQuestoes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Estudos\Faculdade\codes\.vscode\Threads\Provas antigas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDC6369C-E6FD-4DFC-A852-3CD2959AC61D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A800B87D-4BD7-4825-9C37-F49356CF3277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6EA752E0-E1F0-4D20-AE99-72217FC8726F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
@@ -68,10 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="78">
-  <si>
-    <t>Numero</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="95">
   <si>
     <t>Texto</t>
   </si>
@@ -116,9 +113,6 @@
   </si>
   <si>
     <t>2022.2</t>
-  </si>
-  <si>
-    <t>Mecanismos de exclusão mútua podem ser implementados pelo sistema operacional usando as técnicas de desabilitação de interrupção e spin lock . Explique cada uma destas técnicas e indique as vantagens e desvantagens (2,5);</t>
   </si>
   <si>
     <t>A interrupção é considerada o elo entre hardware-software. Qual a importância de interrupções para o gerenciamento do sistema operacional? Explique no contexto de escalonamento e interrupções de relógio (timer) (2,5);</t>
@@ -387,12 +381,269 @@
     <t>- Mutex
 - Exclusão mútua</t>
   </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>A desabilitação de interrupções é uma forma realizar a exclusão mútua impedindo que o escalonador continue a execução de qualquer outro processo ou thread enquanto um deles estiver acessando a região crítica. Essa abordagem de exclusão mútua não funciona para sistemas multiprocessadores visto que a interrupção seria desabilitada em apenas um dos processadores. Dessa forma, os outros poderiam acessar a região crítica de livremente, ou seja, não ocorre exclusão mútua corretamente.</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Resolvida</t>
+  </si>
+  <si>
+    <t>Pendente</t>
+  </si>
+  <si>
+    <t>Aula</t>
+  </si>
+  <si>
+    <t>06_Concorrencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Quando um processo é interrompido, seja por um evento de E/S, uma interrupção de tempo ou outra razão, o sistema operacional precisa salvar o estado atual do processo para que ele possa ser retomado posteriormente. Esse salvamento inclui o program counter (PC), registros da CPU e outras informações de estado. 
+  Quando o escalonador decide que um processo deve ser executado, ele carrega o contexto previamente salvo desse processo. Isso permite que o processo continue sua execução do ponto exato em que foi interrompido, garantindo a continuidade da sua operação. 
+  Ainda, o escalonador usa o contexto do processo para tomar decisões sobre qual processo deve ser o próximo executado. Isso pode incluir as informações sobre prioridade, tempo de CPU e estado, presentes no contexto.</t>
+  </si>
+  <si>
+    <t>aula9-escalonamento
+03_Introducao_2</t>
+  </si>
+  <si>
+    <t>02_Introducao_1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">O funcionamento do bootloader pode ser dividido em duas etapas principais. 
+	Na primeira etapa, após a inicialização do hardware e o POST (Power-On Self-Test), o BIOS busca o código do bootloader no MBR (Master Boot Record), carrega, geralmente, seus primeiros 512 bytes para a memória e transfere o controle para ele. Esta etapa configura o ambiente inicial necessário para a execução do bootloader.
+	Na segunda etapa, com o controle transferido para o bootloader, ele agora deve localizar e carregar o kernel do sistema operacional na memória. O bootloader configura o modo de operação adequado (por exemplo, protected mode), localiza o kernel no sistema de arquivos, carrega-o na memória e, finalmente, transfere o controle para o kernel, iniciando a execução do sistema operacional.
+Para a implementação do bootloader, alguns cuidados são essenciais. O bootloader deve ser </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pequeno o suficiente para caber nos 512 bytes do MBR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. É importante implementar verificações para</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> lidar com falhas na inicialização</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ou problemas de leitura, garantindo uma gestão robusta de erros. O bootloader deve ser </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>compatível com o sistema de arquivos</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>disco onde o kernel está armazenado</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Além disso, a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>segurança</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> é um aspecto crucial, sendo necessário </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>verificar a integridade do código</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> para prevenir execuções maliciosas.</t>
+    </r>
+  </si>
+  <si>
+    <t>Mecanismos de exclusão mútua podem ser implementados pelo sistema operacional usando as técnicas de desabilitação de interrupção e spin lock. Explique cada uma destas técnicas e indique as vantagens e desvantagens (2,5);</t>
+  </si>
+  <si>
+    <r>
+      <t>Definição</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: é uma maneira de implementar exclusão mútua (mutex) por meio de checagens repetidas como um loop (spin) da variável lock que indica se a região crítica pode ou não ser acessada no momento pelo processo/thread que tenta. Quando uma thread quer acessar uma região protegida pelo mutex, tenta adquirir o lock e, enquanto não conseguir, continua checando. Ao conseguir adquirir o lock, acessa a região crítica e segue com a execução. Após concluir as operações na região crítica, libera o lock para que outras threads possam tentar adquirir. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vantagens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Mesmo que ocasione na espera ocupada de processos/threads, pode ser eficiente em operações que fazem uso da região crítica por um curto período de tempo e pelo fato de não requererem mudança de contexto. Além disso, é uma implementação de exclusão mútua que funciona com sistemas multiprocessadores visto que todos os processadores podem checar o mesmo lock. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Desvantagens</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: As threads/processos esperando pelo lock ficam em espera ocupada, fato que desperdiça tempo e processamento da CPU principalmente em processos com muitas threads esperando pelo mesmo lock para prosseguir.</t>
+    </r>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Há 4 condições necessárias mas não suficientes para a ocorrência de deadlocks:
+1. Exclusão mútua
+    Presença de recursos compartilhados em que apenas um processo/thread pode acessar simultaneamente.
+    Prevenção: Técnica de Spooling em que a requisição fica armazenada em disco e quando o recurso estiver disponível o acesso é concebido ao processo/thread que estava esperando.
+2. Posse e espera
+    A possibilidade de adquirir um recurso (posse) e esperar por outro caso ele esteja sendo usado por outro processo/thread
+    Prevenção: Reserva de todos os recursos necessários antes de travar ou não reservar nada, o que deve ser feito com cuidado.
+3. Não preemptividade
+    Dada a posse de um recurso compartilhado para um processo/thread, nenhum outro pode roubá-la, retirar essa posse à força do processo que a possui, só pode ser liberada pelo processo que tem a posse.
+    Prevenção: Permitir que um processo/thread “roube temporariamente”, pegue à força um recurso de outro, o que também deve ser feito com cuidado
+4. Espera circular
+    Há um ciclo fechado de processos e recursos, onde cada processo está esperando por um recurso que o próximo processo na sequência tem posse. Isso continua até que o último processo está esperando por um recurso que o primeiro processo tem a posse.
+    Prevenção: Ordenação numérica dos recursos para evitar uma dada ordem em que ocorre o deadlock, evitando que um processo/thread tente usar um recurso compartilhado ao mesmo tempo que outro.</t>
+  </si>
+  <si>
+    <t>aula10-deadlock</t>
+  </si>
+  <si>
+    <t>aula4-conceitos_adicionais</t>
+  </si>
+  <si>
+    <t>Interrupções de relógio são um tipo de interrupção de hardware que são feitas como uma forma de chamar atenção da CPU para o sinal de interrupção interpretado pelo tratador de interrupções com o objetivo de executar atividades de gerenciamento do sistema operacional. Uma delas é o escalonamento. Para cada processo/thread são definidos fatias de tempo (quantums). A cada interrupção de relógio é verificado se ele acabou. Se sim, o processo é suspenso e e o escalonador passa a executar outro.</t>
+  </si>
+  <si>
+    <t>As chamadas ao sistema são interfaces que permitem que programas solicitem serviços do kernel do sistema operacional. São geradas por meio de interrupções síncronas (traps) que desviam a execução do modo usuário para o modo kernel (núcleo). Ao terminar a execução gerada pelo código da interrupção interpretado pelo tratador de interrupções, o processo anteriormente interrompido volta a ser executado normalmente</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,6 +676,21 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -446,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -463,11 +729,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor theme="2"/>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -483,17 +784,13 @@
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF75BD92"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -575,15 +872,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{602F16FD-8788-4D16-9A52-DA61EB9C7F66}" name="Tabela1" displayName="Tabela1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
-  <autoFilter ref="A1:F43" xr:uid="{602F16FD-8788-4D16-9A52-DA61EB9C7F66}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{F5E11782-C182-4AC0-993D-7F2D51A34A39}" name="Semestre" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{0694AE4C-A66C-4807-A297-755B318D59FD}" name="Numero" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{F820EDCE-94C3-4B88-8D3A-23534F0555CC}" name="Tópicos" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{64EDEF0F-2D09-44D8-8930-E71FEEEF7925}" name="Texto" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{BF61CC40-E408-429C-A95F-D6E3599B2BAF}" name="Resposta" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{97FBD520-9588-4712-A5E6-F9AD7236C2A4}" name="Complemento ao texto" dataDxfId="5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{602F16FD-8788-4D16-9A52-DA61EB9C7F66}" name="Tabela1" displayName="Tabela1" ref="A1:H43" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="A1:H43" xr:uid="{602F16FD-8788-4D16-9A52-DA61EB9C7F66}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{F5E11782-C182-4AC0-993D-7F2D51A34A39}" name="Semestre" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{0694AE4C-A66C-4807-A297-755B318D59FD}" name="N" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{F820EDCE-94C3-4B88-8D3A-23534F0555CC}" name="Tópicos" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{64EDEF0F-2D09-44D8-8930-E71FEEEF7925}" name="Texto" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{BF61CC40-E408-429C-A95F-D6E3599B2BAF}" name="Resposta" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{97FBD520-9588-4712-A5E6-F9AD7236C2A4}" name="Complemento ao texto" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{80583910-433B-41C9-BE38-F2555A1BD7DB}" name="Status" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{A1BA32E6-2727-477E-8F2A-9F6CDF3ACE67}" name="Aula" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -906,638 +1205,870 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DE9F26-DDE6-4C49-B717-D430C96A519E}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C38" sqref="C1:C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="13.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="79.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="40.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" style="1" hidden="1"/>
-    <col min="8" max="16384" width="13.140625" style="1" hidden="1"/>
+    <col min="1" max="1" width="9.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="40.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="13.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="195" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="1">
         <v>5</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="270" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="B7" s="1">
         <v>1</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="1">
         <v>3</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1">
         <v>4</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>5</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1">
         <v>1</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1">
         <v>3</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C14" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1">
         <v>4</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1">
         <v>5</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="F16" s="1" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+      <c r="G16" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="210" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>2</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B19" s="1">
         <v>3</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>4</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1">
         <v>5</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="285" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>6</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1">
         <v>2</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B25" s="1">
         <v>3</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1">
         <v>4</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="240" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1">
         <v>5</v>
       </c>
-      <c r="C27" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>50</v>
+      <c r="C27" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C28" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" s="1">
         <v>2</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>56</v>
+        <v>11</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="F29" s="1" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G29" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30" s="1">
         <v>3</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B31" s="1">
         <v>4</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="215.25" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="300" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B32" s="1">
         <v>5</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1">
         <v>1</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B34" s="1">
         <v>2</v>
       </c>
-      <c r="C34" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C34" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B35" s="1">
         <v>3</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B36" s="1">
         <v>4</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="330" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B37" s="1">
         <v>5</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="195" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="300" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B38" s="1">
         <v>6</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="345" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="180" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
       </c>
+      <c r="C39" s="4"/>
       <c r="D39" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="E39" s="2"/>
-    </row>
-    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B40" s="1">
         <v>2</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C40" s="4"/>
+      <c r="D40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B41" s="1">
         <v>3</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C41" s="4"/>
+      <c r="D41" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B42" s="1">
         <v>4</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="C42" s="4"/>
+      <c r="D42" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="405" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B43" s="1">
         <v>5</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>74</v>
+      <c r="C43" s="4"/>
+      <c r="D43" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="G1:G1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Resolvida">
+      <formula>NOT(ISERROR(SEARCH("Resolvida",G1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>